<commit_message>
Color Scale min and max
</commit_message>
<xml_diff>
--- a/Chapter-12_Excel/reviews-sample.xlsx
+++ b/Chapter-12_Excel/reviews-sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aline\Desktop\Vandeilson_UNICSUL\git_repositorio\python_automate_boring_stuff_exercises\Chapter-12_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1827F081-E96B-43A5-ABAF-0179B6BC733C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1DE306-166A-4B71-9ABC-0170FC75767F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1507,29 +1507,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="15"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -6553,9 +6531,14 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:O100">
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>$H1&lt;3</formula>
+  <conditionalFormatting sqref="H2:H100">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color indexed="37"/>
+        <color indexed="58"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>